<commit_message>
Atnaujintas Excel: panels.xlsx duomenys atnaujinti (Nesilenkia ir kiti pakeitimai)
</commit_message>
<xml_diff>
--- a/static/panels.xlsx
+++ b/static/panels.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulinciu_nemusa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulinciu_nemusa/skaiciuoklev2/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B93A80E4-8571-BC41-8E1B-E83E6C9D8E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53305D3F-1EC1-EF4C-9DA1-EC1898BEC70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8480" yWindow="2000" windowWidth="29920" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>P1 LEDTITGO</t>
   </si>
   <si>
-    <t>P2 Curved</t>
-  </si>
-  <si>
     <t>P2 XR</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>0.07</t>
+  </si>
+  <si>
+    <t>P1 CURVED</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="C5:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -681,27 +681,27 @@
         <v>12.5</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="E7" s="2">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="F7" s="2">
         <v>0.5</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>192</v>
@@ -758,10 +758,10 @@
         <v>6.3</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="M8" s="4">
         <v>0.11</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2">
         <v>192</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
         <v>128</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2">
         <v>128</v>
@@ -890,7 +890,7 @@
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="2">
         <v>128</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="2">
         <v>128</v>
@@ -959,16 +959,16 @@
         <v>10</v>
       </c>
       <c r="M13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="O13" s="5"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2">
         <v>128</v>
@@ -992,10 +992,10 @@
         <v>9</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M14" s="4">
         <v>0.16</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2">
         <v>104</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2">
         <v>104</v>
@@ -1070,10 +1070,10 @@
         <v>9</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M16" s="4">
         <v>0.16</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2">
         <v>84</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2">
         <v>80</v>
@@ -1148,22 +1148,22 @@
         <v>7.95</v>
       </c>
       <c r="K18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="N18" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="O18" s="5"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2">
         <v>256</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2">
         <v>128</v>

</xml_diff>